<commit_message>
ass1P2 pricing problem #soclose
</commit_message>
<xml_diff>
--- a/Assignment 1P2/Bpr_EXAMPLE.xlsx
+++ b/Assignment 1P2/Bpr_EXAMPLE.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03512716-AEAA-4B67-A25E-DD4B28EDE68A}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{074ADE08-DE36-422A-9A3E-3FCC07518160}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -335,14 +335,14 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -366,12 +366,12 @@
         <v>0</v>
       </c>
       <c r="I1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -392,15 +392,15 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="I2">
-        <v>0.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -424,12 +424,12 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -453,12 +453,12 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -482,12 +482,12 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -511,12 +511,12 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -540,12 +540,12 @@
         <v>0</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -569,7 +569,7 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>